<commit_message>
updated mp settings file
</commit_message>
<xml_diff>
--- a/korbinian/examples/settings/korbinian_run_settings_schweris_mp.xlsx
+++ b/korbinian/examples/settings/korbinian_run_settings_schweris_mp.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="200">
-  <si>
-    <t>uniprot_list</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="194">
   <si>
     <t>protein_lists</t>
   </si>
@@ -42,12 +39,6 @@
     <t>The proteins to be analysed are grouped in a numbered list.</t>
   </si>
   <si>
-    <t>For comparing two or more protein lists.</t>
-  </si>
-  <si>
-    <t>Here you can name the protein lists that you are analysing.</t>
-  </si>
-  <si>
     <t>If "TRUE", a list of accessions downloaded from uniprot will be compared against UniRef clusters (e.g. UniRef50, each &gt;50% amino acid identity), and a nonredundant list will be created, using the UniRef "reference sequence" if available. A uniprot flatfile containing the proteins of interest will be created from this list of non-redundant proteins (e.g. List##_selected_flatfile.txt), by copying the records from a larger flatfile (e.g. all membrane proteins). Leave "FALSE" if the selected UniProt flatfile already exists, for example if it has been downloaded directly from UniProt.</t>
   </si>
   <si>
@@ -75,9 +66,6 @@
     <t>If "TRUE", two or more protein lists will be compared (e.g. single-pass vs multi-pass), and a number of figures created and saved.</t>
   </si>
   <si>
-    <t>OLD fuctions, not currently in use</t>
-  </si>
-  <si>
     <t>overwrite_selected_ff</t>
   </si>
   <si>
@@ -297,9 +285,6 @@
     <t>TMD/nonTMD conservation plotting run settings</t>
   </si>
   <si>
-    <t>Old run settings</t>
-  </si>
-  <si>
     <t>run_parse_large_flatfile_with_list_uniprot_accessions</t>
   </si>
   <si>
@@ -309,9 +294,6 @@
     <t>run_create_csv_from_uniprot_flatfile</t>
   </si>
   <si>
-    <t>run_retrieve_simap_feature_table_and_homologues_from_list_in_csv</t>
-  </si>
-  <si>
     <t>run_parse_simap_to_csv</t>
   </si>
   <si>
@@ -330,30 +312,12 @@
     <t>run_compare_lists</t>
   </si>
   <si>
-    <t>old_calculate_TMD_conservation</t>
-  </si>
-  <si>
-    <t>old_calculate_TMD_conservation_by_gappedIdentity</t>
-  </si>
-  <si>
-    <t>old_calculate_TMD_conservation_moment</t>
-  </si>
-  <si>
-    <t>old_conduct_stat_analysis_with_all_seqs_or_nonredundant_seqs</t>
-  </si>
-  <si>
-    <t>old_fix_dfout05_simapcsv_by_adding_query_md5</t>
-  </si>
-  <si>
     <t>parameter</t>
   </si>
   <si>
     <t>1p_min_n_hits_for_data_analysis</t>
   </si>
   <si>
-    <t>old_run_stat_analysis_sim_ratios_in_dfout05</t>
-  </si>
-  <si>
     <t>stat_analysis_all_seqs_or_nonred_seqs</t>
   </si>
   <si>
@@ -510,9 +474,6 @@
     <t>OMPdb_parse_OMPdb_all_selected_to_csv</t>
   </si>
   <si>
-    <t>OMPdb_get_omp_TM_indices_and_slice_from_summary_table</t>
-  </si>
-  <si>
     <t>Protein list settings (UniProt/OMPdb)</t>
   </si>
   <si>
@@ -525,9 +486,6 @@
     <t>If true, the list of failed downloads (e.g. "D:\Databases\main\summaries\05\List05_failed_downloads.txt") will be ignored, and download will be attempted anyway.</t>
   </si>
   <si>
-    <t>slice_TMDs_from_homologues</t>
-  </si>
-  <si>
     <t>If "TRUE", the homologues for each TMD will be sliced out of the query, match and markup sequences from the SIMAP data. This is necessary for both the create_fasta or calculate_AAIMON_ratios.</t>
   </si>
   <si>
@@ -616,6 +574,30 @@
   </si>
   <si>
     <t>download_feature_tables</t>
+  </si>
+  <si>
+    <t>simap_dir</t>
+  </si>
+  <si>
+    <t>D:\Databases\simap</t>
+  </si>
+  <si>
+    <t>run_download_homologues</t>
+  </si>
+  <si>
+    <t>OMPdb_get_TM_indices_and_slice</t>
+  </si>
+  <si>
+    <t>protein_list_number</t>
+  </si>
+  <si>
+    <t>Only for comparing two or more protein lists.</t>
+  </si>
+  <si>
+    <t>Only for comparing two or more protein lists. Here you can name the protein lists that you are analysing.</t>
+  </si>
+  <si>
+    <t>run_slice_TMDs_from_homologues</t>
   </si>
 </sst>
 </file>
@@ -992,7 +974,105 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="58">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1607,69 +1687,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="52.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="4" customWidth="1"/>
     <col min="3" max="3" width="85.5703125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="53"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="B3" s="37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>8</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>9</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="62" customFormat="1" x14ac:dyDescent="0.25">
@@ -1677,53 +1757,53 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="27"/>
     </row>
     <row r="8" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B8" s="70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="B9" s="70">
         <v>16</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1732,91 +1812,91 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="B13" s="39"/>
       <c r="C13" s="55"/>
     </row>
     <row r="14" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B14" s="70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="56"/>
     </row>
     <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B15" s="70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="68"/>
     </row>
     <row r="16" spans="1:3" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="B16" s="70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="32"/>
     </row>
     <row r="17" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B17" s="70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="56" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B18" s="70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="68" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="B19" s="70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B20" s="70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="56" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B21" s="70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1825,31 +1905,31 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B23" s="41"/>
       <c r="C23" s="57"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="64" t="s">
-        <v>97</v>
+        <v>188</v>
       </c>
       <c r="B24" s="70" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="65" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="66" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B25" s="70" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="66" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1858,64 +1938,64 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B27" s="43"/>
       <c r="C27" s="59"/>
     </row>
     <row r="28" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
       <c r="B28" s="70" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="B29" s="70" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B30" s="70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="B31" s="70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B32" s="70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1925,230 +2005,157 @@
     </row>
     <row r="34" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B34" s="45"/>
       <c r="C34" s="60"/>
     </row>
     <row r="35" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B35" s="70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" s="61" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B36" s="70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" s="61" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B37" s="70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C37" s="61" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="62"/>
       <c r="C38" s="62"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="B39" s="48"/>
-      <c r="C39" s="27"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="B40" s="70" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="B41" s="70" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="B42" s="70" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="B43" s="70" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="B44" s="70" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="B45" s="70" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B6 B46:B1048576">
-    <cfRule type="containsText" dxfId="43" priority="388" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="B1 B6 B39:B1048576">
+    <cfRule type="containsText" dxfId="57" priority="441" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="containsText" dxfId="42" priority="386" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="56" priority="439" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="containsText" dxfId="41" priority="385" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="55" priority="438" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="containsText" dxfId="40" priority="384" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="54" priority="437" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="containsText" dxfId="39" priority="383" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="53" priority="436" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B38)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B40:B45 B35 B37 B17:B18">
-    <cfRule type="containsText" dxfId="38" priority="382" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="B35 B37 B17:B18">
+    <cfRule type="containsText" dxfId="52" priority="435" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="containsText" dxfId="37" priority="372" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="51" priority="425" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="36" priority="306" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="50" priority="359" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B11">
-    <cfRule type="containsText" dxfId="35" priority="191" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="49" priority="244" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="containsText" dxfId="34" priority="190" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="48" priority="243" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="containsText" dxfId="33" priority="78" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="47" priority="131" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="containsText" dxfId="32" priority="65" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="46" priority="118" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="containsText" dxfId="30" priority="45" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="45" priority="98" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="29" priority="35" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="44" priority="88" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="43" priority="86" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31">
-    <cfRule type="containsText" dxfId="27" priority="20" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="26" priority="15" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="42" priority="37" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="containsText" dxfId="20" priority="9" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="40" priority="24" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="39" priority="23" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B21)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24">
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B24)))</formula>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="containsText" dxfId="29" priority="15" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31">
+    <cfRule type="containsText" dxfId="27" priority="14" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="23" priority="12" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="containsText" dxfId="21" priority="11" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
@@ -2168,10 +2175,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2183,113 +2190,121 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="55"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>152</v>
-      </c>
-      <c r="B8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="A8" s="18" t="s">
         <v>153</v>
       </c>
+      <c r="B8" s="39"/>
+      <c r="C8" s="55"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>160</v>
-      </c>
-      <c r="B9" s="70" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>161</v>
+        <v>140</v>
+      </c>
+      <c r="B9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>190</v>
+        <v>148</v>
       </c>
       <c r="B10" s="70" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>161</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B9)))</formula>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B10)))</formula>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2301,8 +2316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,34 +2329,34 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="53"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="54"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B4" s="37">
         <v>50</v>
@@ -2350,24 +2365,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2376,41 +2391,41 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="55"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="56"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="56"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="56"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B12" s="40" t="b">
         <v>0</v>
@@ -2419,27 +2434,27 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="56"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B14" s="40">
         <v>1000</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B15" s="40">
         <v>1.0000000000000001E-5</v>
@@ -2448,7 +2463,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B16" s="40">
         <v>5000</v>
@@ -2457,7 +2472,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B17" s="40">
         <v>3000</v>
@@ -2466,21 +2481,21 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="56" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C19" s="56"/>
     </row>
@@ -2490,67 +2505,67 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="76" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B21" s="77"/>
       <c r="C21" s="78"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="79" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B22" s="80" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="81"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="79" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B23" s="80" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="81"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="79" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="B24" s="80" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" s="81"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="79" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B25" s="80" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C25" s="81"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="79" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="B26" s="80">
         <v>10</v>
       </c>
       <c r="C26" s="81" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="79" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B27" s="80">
         <v>10</v>
       </c>
       <c r="C27" s="81" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2559,67 +2574,67 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="57"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="58" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B31" s="42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="58" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B32" s="42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33" s="58"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B34" s="42">
         <v>60</v>
       </c>
       <c r="C34" s="58" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="B35" s="42">
         <v>10</v>
@@ -2628,7 +2643,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B36" s="42">
         <v>10</v>
@@ -2637,64 +2652,64 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B37" s="42" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B38" s="42">
         <v>0.4</v>
       </c>
       <c r="C38" s="58" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B39" s="42">
         <v>1</v>
       </c>
       <c r="C39" s="58" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B40" s="42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40" s="58"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B41" s="42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41" s="58"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B42" s="42" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C42" s="58" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2703,36 +2718,36 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="71" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B44" s="72"/>
       <c r="C44" s="73"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="74" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B45" s="75" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" s="75" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="74" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B46" s="75" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C46" s="75" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="74" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B47" s="75">
         <v>2</v>
@@ -2743,7 +2758,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="74" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B48" s="75">
         <v>2</v>
@@ -2754,7 +2769,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="74" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B49" s="75">
         <v>0.7</v>
@@ -2765,7 +2780,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="74" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B50" s="75">
         <v>1</v>
@@ -2776,7 +2791,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="74" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B51" s="75">
         <v>0.2</v>
@@ -2787,7 +2802,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="74" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B52" s="75">
         <v>0.2</v>
@@ -2798,18 +2813,18 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="74" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B53" s="75" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C53" s="75" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="74" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B54" s="75">
         <v>20</v>
@@ -2820,18 +2835,18 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="74" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B55" s="75" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C55" s="75" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="74" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B56" s="75">
         <v>1.1000000000000001</v>
@@ -2842,35 +2857,35 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="74" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="B57" s="75">
         <v>0</v>
       </c>
       <c r="C57" s="75" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="74" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="B58" s="75">
         <v>0</v>
       </c>
       <c r="C58" s="75" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="74" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B59" s="75" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C59" s="75" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2879,23 +2894,23 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B61" s="43"/>
       <c r="C61" s="59"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B62" s="44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C62" s="25"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B63" s="44">
         <v>2</v>
@@ -2904,7 +2919,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B64" s="44">
         <v>24</v>
@@ -2913,7 +2928,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B65" s="44">
         <v>20</v>
@@ -2926,14 +2941,14 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B67" s="45"/>
       <c r="C67" s="60"/>
     </row>
     <row r="68" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B68" s="46">
         <v>30</v>
@@ -2942,16 +2957,16 @@
     </row>
     <row r="69" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B69" s="46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C69" s="61"/>
     </row>
     <row r="70" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B70" s="46">
         <v>3.05</v>
@@ -2960,7 +2975,7 @@
     </row>
     <row r="71" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="21" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B71" s="46">
         <v>20</v>
@@ -2969,7 +2984,7 @@
     </row>
     <row r="72" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B72" s="46">
         <v>31</v>
@@ -2978,25 +2993,25 @@
     </row>
     <row r="73" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B73" s="46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C73" s="61"/>
     </row>
     <row r="74" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B74" s="46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C74" s="61"/>
     </row>
     <row r="75" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B75" s="46">
         <v>0.05</v>
@@ -3005,7 +3020,7 @@
     </row>
     <row r="76" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B76" s="46">
         <v>3</v>
@@ -3014,16 +3029,16 @@
     </row>
     <row r="77" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B77" s="46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C77" s="61"/>
     </row>
     <row r="78" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B78" s="46">
         <v>1.4550000000000001</v>
@@ -3032,7 +3047,7 @@
     </row>
     <row r="79" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B79" s="46">
         <v>31</v>
@@ -3041,16 +3056,16 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B80" s="46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C80" s="61"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="21" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B81" s="46">
         <v>0.55500000000000005</v>
@@ -3059,7 +3074,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="21" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B82" s="46">
         <v>0.5</v>
@@ -3068,7 +3083,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="21" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B83" s="46">
         <v>1.75</v>
@@ -3077,23 +3092,23 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="21" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B84" s="46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C84" s="61"/>
     </row>
     <row r="86" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="26" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B86" s="48"/>
       <c r="C86" s="27"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="28" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B87" s="49">
         <v>0</v>
@@ -3102,7 +3117,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="28" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B88" s="49">
         <v>-12</v>
@@ -3111,7 +3126,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="28" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B89" s="49">
         <v>-2</v>
@@ -3120,16 +3135,16 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B90" s="49" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C90" s="29"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B91" s="49">
         <v>-0.2</v>
@@ -3138,7 +3153,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="28" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B92" s="49">
         <v>-1</v>
@@ -3147,7 +3162,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B93" s="49">
         <v>-1</v>
@@ -3156,7 +3171,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B94" s="49">
         <v>0</v>
@@ -3165,32 +3180,32 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="28" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B95" s="49" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C95" s="29"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="34" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B97" s="50"/>
       <c r="C97" s="30"/>
     </row>
     <row r="98" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B98" s="51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C98" s="33"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B99" s="51">
         <v>5</v>
@@ -3199,25 +3214,25 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B100" s="51" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C100" s="33"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B101" s="51" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C101" s="51"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
created fastagap, a new method to save TMD_seq_plus_surr only for homologues with gaps in the TMD added calculation of hydrophobicity to the slice scripts added filtering by Hessa hydrophilicity to cons_ratio, fasta, and fastagap added filtering by length of nonTMD to cons_ratio added filtering by number of gaps in TMD to cons_ratio replaced several print statements with sys.stdout.write, making it easier to detect print statements added during development
</commit_message>
<xml_diff>
--- a/korbinian/examples/settings/korbinian_run_settings_schweris_mp.xlsx
+++ b/korbinian/examples/settings/korbinian_run_settings_schweris_mp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="3195" windowWidth="14265" windowHeight="7620"/>
+    <workbookView xWindow="3195" yWindow="3375" windowWidth="14265" windowHeight="7440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="run_settings" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="193">
   <si>
     <t>protein_lists</t>
   </si>
@@ -102,9 +102,6 @@
     <t>all</t>
   </si>
   <si>
-    <t>gappedIdentity</t>
-  </si>
-  <si>
     <t>suppress_error_logging_to_console</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>overwrite_previous_gap_analysis</t>
   </si>
   <si>
-    <t>allowed_gaps_per_tmd</t>
-  </si>
-  <si>
     <t>max_number_of_tmds</t>
   </si>
   <si>
@@ -336,39 +330,9 @@
     <t>mp_xlim_max01</t>
   </si>
   <si>
-    <t>fa_database</t>
-  </si>
-  <si>
-    <t>fa_identity_method</t>
-  </si>
-  <si>
     <t>fa_X_allowed_in_sel_seq</t>
   </si>
   <si>
-    <t>cr_database</t>
-  </si>
-  <si>
-    <t>cr_min_identity_of_TMD_initial_filter</t>
-  </si>
-  <si>
-    <t>cr_min_identity_of_TMD_final_filter</t>
-  </si>
-  <si>
-    <t>cr_X_allowed_in_full_seq</t>
-  </si>
-  <si>
-    <t>cr_min_len_query_aln_seq_excl_TMD</t>
-  </si>
-  <si>
-    <t>cr_identity_method</t>
-  </si>
-  <si>
-    <t>cr_maximum_identity_of_full_protein</t>
-  </si>
-  <si>
-    <t>cr_randomised_tmd</t>
-  </si>
-  <si>
     <t>fa_X_allowed_in_full_seq</t>
   </si>
   <si>
@@ -378,12 +342,6 @@
     <t>fa_min_identity_of_full_protein</t>
   </si>
   <si>
-    <t>cr_max_n_gaps_in_match_TMD</t>
-  </si>
-  <si>
-    <t>cr_max_n_gaps_in_query_TMD</t>
-  </si>
-  <si>
     <t>fa_max_n_gaps_in_match_TMD</t>
   </si>
   <si>
@@ -408,24 +366,12 @@
     <t>SIMAP homologue filtering for fasta (fa) output</t>
   </si>
   <si>
-    <t>filter_selected_seq_based_on_hydrophobicity</t>
-  </si>
-  <si>
-    <t>max_hydrophilicity_Hessa</t>
-  </si>
-  <si>
-    <t>maximum hydrophilicity of the selected sequence (BUT NOT THE SURROUNDING SEQ!). Hydrophobicity is calculated with Hessa scale, negative value means favourable membrane insertion. Seqs that have mean hydrophobicity score above the cutoff will be excluded from the alignment.</t>
-  </si>
-  <si>
     <t>your_name</t>
   </si>
   <si>
     <t>ASCII text! Identifier to determine who downloaded SIMAP homologues</t>
   </si>
   <si>
-    <t>not used!</t>
-  </si>
-  <si>
     <t>0.4 = 40% aa identity excluding gaps</t>
   </si>
   <si>
@@ -549,15 +495,6 @@
     <t>analyse_signal_peptides</t>
   </si>
   <si>
-    <t>cr_minimum_length_match_sequence</t>
-  </si>
-  <si>
-    <t>cr_minimum_length_non_TMD_sequence</t>
-  </si>
-  <si>
-    <t>not in use</t>
-  </si>
-  <si>
     <t>overwrite_sliced_homologues</t>
   </si>
   <si>
@@ -598,6 +535,66 @@
   </si>
   <si>
     <t>run_slice_TMDs_from_homologues</t>
+  </si>
+  <si>
+    <t>Number of concurrent processes to be run, using multiple CPU cores if available.</t>
+  </si>
+  <si>
+    <t>gap_min_identity_of_full_protein</t>
+  </si>
+  <si>
+    <t>gap_max_identity_of_full_protein</t>
+  </si>
+  <si>
+    <t>gap_min_n_gaps_in_TMD</t>
+  </si>
+  <si>
+    <t>gap_max_n_gaps_in_TMD</t>
+  </si>
+  <si>
+    <t>gap_allowed_gaps_per_tmd</t>
+  </si>
+  <si>
+    <t>run_gather_gap_densities</t>
+  </si>
+  <si>
+    <t>fa_max_n_gaps_in_match_TMD_plus_surr</t>
+  </si>
+  <si>
+    <t>Fasta (fa) output for gap analysis.</t>
+  </si>
+  <si>
+    <t>save_fasta_for_gap_analysis</t>
+  </si>
+  <si>
+    <t>fa_min_n_gaps_in_match_TMD_plus_surr</t>
+  </si>
+  <si>
+    <t>run_fastagap_save</t>
+  </si>
+  <si>
+    <t>cr_max_n_gaps_in_TMD</t>
+  </si>
+  <si>
+    <t>cr_min_len_nonTMD</t>
+  </si>
+  <si>
+    <t>cr_min_identity_of_TMD</t>
+  </si>
+  <si>
+    <t>linked to fa setting above</t>
+  </si>
+  <si>
+    <t>fa_max_hydrophilicity_Hessa</t>
+  </si>
+  <si>
+    <t>maximum hydrophilicity of the selected sequence (BUT NOT THE SURROUNDING SEQ!). Hydrophobicity is calculated with Hessa scale, negative value means favourable membrane insertion. Seqs that have mean hydrophobicity score above the cutoff will be excluded from the alignment. Typically, anything above 12 is unlikely to be a TMD.</t>
+  </si>
+  <si>
+    <t>cr_max_hydrophilicity_Hessa</t>
+  </si>
+  <si>
+    <t>gap_max_hydrophilicity_Hessa</t>
   </si>
 </sst>
 </file>
@@ -793,7 +790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -970,32 +967,17 @@
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="55">
     <dxf>
       <fill>
         <patternFill>
@@ -1687,44 +1669,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="4" customWidth="1"/>
+    <col min="1" max="1" width="49.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="85.5703125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="53"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="B3" s="37">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="C3" s="54" t="s">
         <v>6</v>
@@ -1738,7 +1720,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1749,7 +1731,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="62" customFormat="1" x14ac:dyDescent="0.25">
@@ -1757,53 +1739,53 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="27"/>
     </row>
     <row r="8" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="B8" s="70" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="B9" s="70">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1812,14 +1794,14 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="B13" s="39"/>
       <c r="C13" s="55"/>
     </row>
     <row r="14" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="B14" s="70" t="s">
         <v>5</v>
@@ -1828,7 +1810,7 @@
     </row>
     <row r="15" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="B15" s="70" t="s">
         <v>5</v>
@@ -1837,7 +1819,7 @@
     </row>
     <row r="16" spans="1:3" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="B16" s="70" t="s">
         <v>5</v>
@@ -1846,7 +1828,7 @@
     </row>
     <row r="17" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B17" s="70" t="s">
         <v>5</v>
@@ -1857,7 +1839,7 @@
     </row>
     <row r="18" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18" s="70" t="s">
         <v>5</v>
@@ -1868,7 +1850,7 @@
     </row>
     <row r="19" spans="1:3" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="B19" s="70" t="s">
         <v>5</v>
@@ -1879,7 +1861,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B20" s="70" t="s">
         <v>5</v>
@@ -1890,7 +1872,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="B21" s="70" t="s">
         <v>5</v>
@@ -1905,14 +1887,14 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B23" s="41"/>
       <c r="C23" s="57"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="64" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="B24" s="70" t="s">
         <v>5</v>
@@ -1923,7 +1905,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="66" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B25" s="70" t="s">
         <v>5</v>
@@ -1938,234 +1920,277 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B27" s="43"/>
       <c r="C27" s="59"/>
     </row>
     <row r="28" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="B28" s="70" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="B29" s="70" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B30" s="70" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="B31" s="70" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B32" s="70" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="62"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="62"/>
+      <c r="A33" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="25"/>
     </row>
     <row r="34" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B34" s="45"/>
-      <c r="C34" s="60"/>
+      <c r="A34" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="25"/>
     </row>
     <row r="35" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="61" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="61" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="62"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="62"/>
+    </row>
+    <row r="36" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="45"/>
+      <c r="C36" s="60"/>
+    </row>
+    <row r="37" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B37" s="70" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="61" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="61" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="62"/>
-      <c r="C38" s="62"/>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="62"/>
+      <c r="C40" s="62"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B6 B39:B1048576">
-    <cfRule type="containsText" dxfId="57" priority="441" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="B1 B6 B41:B1048576">
+    <cfRule type="containsText" dxfId="32" priority="634" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="containsText" dxfId="56" priority="439" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="31" priority="632" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="containsText" dxfId="55" priority="438" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="30" priority="631" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B26)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B33">
-    <cfRule type="containsText" dxfId="54" priority="437" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B33)))</formula>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="containsText" dxfId="29" priority="630" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="containsText" dxfId="28" priority="629" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39 B17:B18">
+    <cfRule type="containsText" dxfId="27" priority="628" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="containsText" dxfId="53" priority="436" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="26" priority="618" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B38)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35 B37 B17:B18">
-    <cfRule type="containsText" dxfId="52" priority="435" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
-    <cfRule type="containsText" dxfId="51" priority="425" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="50" priority="359" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="25" priority="552" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B11">
-    <cfRule type="containsText" dxfId="49" priority="244" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="24" priority="437" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="containsText" dxfId="48" priority="243" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="23" priority="436" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="containsText" dxfId="47" priority="131" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="22" priority="324" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="containsText" dxfId="46" priority="118" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="21" priority="311" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
-    <cfRule type="containsText" dxfId="45" priority="98" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="44" priority="88" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="20" priority="281" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="43" priority="86" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="19" priority="279" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="42" priority="37" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="18" priority="230" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="containsText" dxfId="17" priority="124" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25">
+    <cfRule type="containsText" dxfId="16" priority="106" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="40" priority="24" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="15" priority="61" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
-    <cfRule type="containsText" dxfId="39" priority="23" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="containsText" dxfId="29" priority="15" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="containsText" dxfId="27" priority="14" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="14" priority="46" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B31)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25">
-    <cfRule type="containsText" dxfId="23" priority="12" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B25)))</formula>
+  <conditionalFormatting sqref="B33">
+    <cfRule type="containsText" dxfId="13" priority="18" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B33)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24">
-    <cfRule type="containsText" dxfId="21" priority="11" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B24)))</formula>
+  <conditionalFormatting sqref="B37">
+    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="containsText" dxfId="11" priority="15" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2178,7 +2203,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,120 +2215,120 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="55"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="B10" s="70" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2314,10 +2339,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2329,18 +2354,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="53"/>
@@ -2368,10 +2393,10 @@
         <v>18</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2382,7 +2407,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2391,14 +2416,14 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="55"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="40" t="s">
         <v>5</v>
@@ -2416,7 +2441,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="B11" s="40" t="s">
         <v>5</v>
@@ -2443,18 +2468,18 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="40">
         <v>1000</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="40">
         <v>1.0000000000000001E-5</v>
@@ -2463,7 +2488,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="40">
         <v>5000</v>
@@ -2472,7 +2497,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="40">
         <v>3000</v>
@@ -2481,21 +2506,21 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="B18" s="40" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="56" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C19" s="56"/>
     </row>
@@ -2505,14 +2530,14 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="76" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="B21" s="77"/>
       <c r="C21" s="78"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="79" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="B22" s="80" t="s">
         <v>4</v>
@@ -2521,7 +2546,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="79" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="B23" s="80" t="s">
         <v>4</v>
@@ -2530,16 +2555,16 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="79" t="s">
-        <v>144</v>
-      </c>
-      <c r="B24" s="80" t="s">
-        <v>5</v>
+        <v>126</v>
+      </c>
+      <c r="B24" s="82" t="s">
+        <v>4</v>
       </c>
       <c r="C24" s="81"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="79" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="B25" s="80" t="s">
         <v>26</v>
@@ -2548,24 +2573,24 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="79" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="B26" s="80">
         <v>10</v>
       </c>
       <c r="C26" s="81" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="79" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="B27" s="80">
         <v>10</v>
       </c>
       <c r="C27" s="81" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2574,180 +2599,172 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="57"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B30" s="42" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="58" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B31" s="42" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="58" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="B32" s="42" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="B33" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="58"/>
+        <v>189</v>
+      </c>
+      <c r="B33" s="42">
+        <v>12</v>
+      </c>
+      <c r="C33" s="58" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="B34" s="42">
-        <v>60</v>
-      </c>
-      <c r="C34" s="58" t="s">
-        <v>132</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C34" s="58"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B35" s="42">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C35" s="58"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B36" s="42">
-        <v>10</v>
-      </c>
-      <c r="C36" s="58"/>
+        <v>0.8</v>
+      </c>
+      <c r="C36" s="58" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B37" s="42" t="s">
-        <v>28</v>
+        <v>106</v>
+      </c>
+      <c r="B37" s="42">
+        <v>1</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="B38" s="42">
-        <v>0.4</v>
-      </c>
-      <c r="C38" s="58" t="s">
-        <v>136</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B38" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="58"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="B39" s="42">
-        <v>1</v>
-      </c>
-      <c r="C39" s="58" t="s">
-        <v>137</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="B39" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="58"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B40" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="58"/>
+      <c r="A40" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="B40" s="41"/>
+      <c r="C40" s="57"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
-        <v>108</v>
+        <v>182</v>
       </c>
       <c r="B41" s="42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41" s="58"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="B42" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="C42" s="58" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="38"/>
-      <c r="C43" s="8"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="71" t="s">
-        <v>128</v>
-      </c>
-      <c r="B44" s="72"/>
-      <c r="C44" s="73"/>
+        <v>183</v>
+      </c>
+      <c r="B42" s="42">
+        <v>1</v>
+      </c>
+      <c r="C42" s="58"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="B43" s="42">
+        <v>4</v>
+      </c>
+      <c r="C43" s="58"/>
+    </row>
+    <row r="44" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="38"/>
+      <c r="C44" s="8"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="74" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="75" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="75" t="s">
-        <v>4</v>
-      </c>
+      <c r="A45" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" s="72"/>
+      <c r="C45" s="73"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="74" t="s">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="B46" s="75" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C46" s="75" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="74" t="s">
-        <v>120</v>
+        <v>185</v>
       </c>
       <c r="B47" s="75">
         <v>2</v>
@@ -2758,43 +2775,46 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="74" t="s">
-        <v>121</v>
+        <v>191</v>
       </c>
       <c r="B48" s="75">
-        <v>2</v>
-      </c>
-      <c r="C48" s="75">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="C48" s="83" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="74" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="B49" s="75">
-        <v>0.7</v>
-      </c>
-      <c r="C49" s="75">
-        <v>0.4</v>
+        <f>B36</f>
+        <v>0.8</v>
+      </c>
+      <c r="C49" s="83" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="74" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="B50" s="75">
+        <f>B37</f>
         <v>1</v>
       </c>
-      <c r="C50" s="75">
-        <v>1</v>
+      <c r="C50" s="83" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="74" t="s">
-        <v>110</v>
+        <v>187</v>
       </c>
       <c r="B51" s="75">
-        <v>0.2</v>
+        <f>B49-0.4</f>
+        <v>0.4</v>
       </c>
       <c r="C51" s="75">
         <v>0.3</v>
@@ -2802,183 +2822,181 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="74" t="s">
-        <v>111</v>
+        <v>186</v>
       </c>
       <c r="B52" s="75">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="C52" s="75">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="74" t="s">
-        <v>112</v>
-      </c>
-      <c r="B53" s="75" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="75" t="s">
-        <v>5</v>
-      </c>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="38"/>
+      <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="74" t="s">
-        <v>113</v>
-      </c>
-      <c r="B54" s="75">
-        <v>20</v>
-      </c>
-      <c r="C54" s="75">
-        <v>20</v>
-      </c>
+      <c r="A54" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="43"/>
+      <c r="C54" s="59"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="74" t="s">
-        <v>114</v>
-      </c>
-      <c r="B55" s="75" t="s">
-        <v>28</v>
-      </c>
-      <c r="C55" s="75" t="s">
-        <v>28</v>
-      </c>
+      <c r="A55" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="25"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="74" t="s">
-        <v>115</v>
-      </c>
-      <c r="B56" s="75">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C56" s="75">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A56" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B56" s="44">
+        <v>2</v>
+      </c>
+      <c r="C56" s="25"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="74" t="s">
+      <c r="A57" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B57" s="44">
+        <f>B36</f>
+        <v>0.8</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B58" s="44">
+        <f>B37</f>
+        <v>1</v>
+      </c>
+      <c r="C58" s="25" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B59" s="44">
+        <v>1</v>
+      </c>
+      <c r="C59" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B57" s="75">
-        <v>0</v>
-      </c>
-      <c r="C57" s="75" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="74" t="s">
-        <v>178</v>
-      </c>
-      <c r="B58" s="75">
-        <v>0</v>
-      </c>
-      <c r="C58" s="75" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="74" t="s">
-        <v>116</v>
-      </c>
-      <c r="B59" s="75" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="75" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="38"/>
-      <c r="C60" s="8"/>
+      <c r="B60" s="44">
+        <v>2</v>
+      </c>
+      <c r="C60" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="B61" s="43"/>
-      <c r="C61" s="59"/>
+      <c r="A61" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B61" s="44">
+        <v>24</v>
+      </c>
+      <c r="C61" s="25"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B62" s="44" t="s">
-        <v>4</v>
+        <v>50</v>
+      </c>
+      <c r="B62" s="44">
+        <v>20</v>
       </c>
       <c r="C62" s="25"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>50</v>
+        <v>192</v>
       </c>
       <c r="B63" s="44">
-        <v>2</v>
-      </c>
-      <c r="C63" s="25"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B64" s="44">
-        <v>24</v>
-      </c>
-      <c r="C64" s="25"/>
+        <v>12</v>
+      </c>
+      <c r="C63" s="25" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="38"/>
+      <c r="C64" s="8"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B65" s="44">
-        <v>20</v>
-      </c>
-      <c r="C65" s="25"/>
+      <c r="A65" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" s="45"/>
+      <c r="C65" s="60"/>
     </row>
     <row r="66" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="38"/>
-      <c r="C66" s="8"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B67" s="45"/>
-      <c r="C67" s="60"/>
+      <c r="A66" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B66" s="46">
+        <v>30</v>
+      </c>
+      <c r="C66" s="61"/>
+    </row>
+    <row r="67" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="61"/>
     </row>
     <row r="68" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
         <v>73</v>
       </c>
       <c r="B68" s="46">
-        <v>30</v>
+        <v>3.05</v>
       </c>
       <c r="C68" s="61"/>
     </row>
     <row r="69" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B69" s="46" t="s">
-        <v>4</v>
+        <v>97</v>
+      </c>
+      <c r="B69" s="46">
+        <v>20</v>
       </c>
       <c r="C69" s="61"/>
     </row>
     <row r="70" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B70" s="46">
-        <v>3.05</v>
+        <v>31</v>
       </c>
       <c r="C70" s="61"/>
     </row>
     <row r="71" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B71" s="46">
-        <v>20</v>
+        <v>75</v>
+      </c>
+      <c r="B71" s="46" t="s">
+        <v>4</v>
       </c>
       <c r="C71" s="61"/>
     </row>
@@ -2986,8 +3004,8 @@
       <c r="A72" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B72" s="46">
-        <v>31</v>
+      <c r="B72" s="46" t="s">
+        <v>5</v>
       </c>
       <c r="C72" s="61"/>
     </row>
@@ -2995,8 +3013,8 @@
       <c r="A73" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B73" s="46" t="s">
-        <v>4</v>
+      <c r="B73" s="46">
+        <v>0.05</v>
       </c>
       <c r="C73" s="61"/>
     </row>
@@ -3004,8 +3022,8 @@
       <c r="A74" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B74" s="46" t="s">
-        <v>5</v>
+      <c r="B74" s="46">
+        <v>3</v>
       </c>
       <c r="C74" s="61"/>
     </row>
@@ -3013,8 +3031,8 @@
       <c r="A75" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B75" s="46">
-        <v>0.05</v>
+      <c r="B75" s="46" t="s">
+        <v>4</v>
       </c>
       <c r="C75" s="61"/>
     </row>
@@ -3023,7 +3041,7 @@
         <v>80</v>
       </c>
       <c r="B76" s="46">
-        <v>3</v>
+        <v>1.4550000000000001</v>
       </c>
       <c r="C76" s="61"/>
     </row>
@@ -3031,208 +3049,190 @@
       <c r="A77" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="B77" s="46" t="s">
-        <v>4</v>
+      <c r="B77" s="46">
+        <v>31</v>
       </c>
       <c r="C77" s="61"/>
     </row>
-    <row r="78" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="B78" s="46">
-        <v>1.4550000000000001</v>
+      <c r="B78" s="46" t="s">
+        <v>5</v>
       </c>
       <c r="C78" s="61"/>
     </row>
-    <row r="79" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="21" t="s">
         <v>83</v>
       </c>
       <c r="B79" s="46">
-        <v>31</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="C79" s="61"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B80" s="46" t="s">
-        <v>5</v>
+        <v>102</v>
+      </c>
+      <c r="B80" s="46">
+        <v>0.5</v>
       </c>
       <c r="C80" s="61"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="21" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="B81" s="46">
-        <v>0.55500000000000005</v>
+        <v>1.75</v>
       </c>
       <c r="C81" s="61"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="B82" s="46">
-        <v>0.5</v>
+        <v>25</v>
+      </c>
+      <c r="B82" s="46" t="s">
+        <v>4</v>
       </c>
       <c r="C82" s="61"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="B83" s="46">
-        <v>1.75</v>
-      </c>
-      <c r="C83" s="61"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B84" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="C84" s="61"/>
-    </row>
-    <row r="86" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B86" s="48"/>
-      <c r="C86" s="27"/>
+    <row r="84" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B84" s="48"/>
+      <c r="C84" s="27"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B85" s="49">
+        <v>0</v>
+      </c>
+      <c r="C85" s="29"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B86" s="49">
+        <v>-12</v>
+      </c>
+      <c r="C86" s="29"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B87" s="49">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C87" s="29"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B88" s="49">
-        <v>-12</v>
+        <v>35</v>
+      </c>
+      <c r="B88" s="49" t="s">
+        <v>40</v>
       </c>
       <c r="C88" s="29"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B89" s="49">
-        <v>-2</v>
+        <v>-0.2</v>
       </c>
       <c r="C89" s="29"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B90" s="49" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="B90" s="49">
+        <v>-1</v>
       </c>
       <c r="C90" s="29"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B91" s="49">
-        <v>-0.2</v>
+        <v>-1</v>
       </c>
       <c r="C91" s="29"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B92" s="49">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C92" s="29"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B93" s="49">
-        <v>-1</v>
+        <v>101</v>
+      </c>
+      <c r="B93" s="49" t="s">
+        <v>41</v>
       </c>
       <c r="C93" s="29"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B94" s="49">
-        <v>0</v>
-      </c>
-      <c r="C94" s="29"/>
-    </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="B95" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="C95" s="29"/>
+      <c r="A95" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B95" s="50"/>
+      <c r="C95" s="30"/>
+    </row>
+    <row r="96" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B96" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="33"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="B97" s="50"/>
-      <c r="C97" s="30"/>
-    </row>
-    <row r="98" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B97" s="51">
+        <v>5</v>
+      </c>
+      <c r="C97" s="33"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B98" s="51" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C98" s="33"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B99" s="51">
-        <v>5</v>
-      </c>
-      <c r="C99" s="33"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B100" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="C100" s="33"/>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B101" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="B99" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C101" s="51"/>
+      <c r="C99" s="51"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
major update to fastagap, including calculation of gap positions, organising of indices, and saving of final pickle file with all gap positions
</commit_message>
<xml_diff>
--- a/korbinian/examples/settings/korbinian_run_settings_schweris_mp.xlsx
+++ b/korbinian/examples/settings/korbinian_run_settings_schweris_mp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="3375" windowWidth="14265" windowHeight="7440" activeTab="2"/>
+    <workbookView xWindow="3195" yWindow="3375" windowWidth="14265" windowHeight="7440"/>
   </bookViews>
   <sheets>
     <sheet name="run_settings" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="194">
   <si>
     <t>protein_lists</t>
   </si>
@@ -595,6 +595,9 @@
   </si>
   <si>
     <t>gap_max_hydrophilicity_Hessa</t>
+  </si>
+  <si>
+    <t>maximum hydrophilicity of the selected sequence (BUT NOT THE SURROUNDING SEQ!). Hydrophobicity is calculated with Hessa scale, negative value means favourable membrane insertion. Seqs that have mean hydrophobicity score above the cutoff will be excluded from the alignment. Typically, anything above 12 is unlikely to be a TMD for alpha helical proteins, and above 30 for beta-barrel proteins.</t>
   </si>
 </sst>
 </file>
@@ -790,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -973,11 +976,28 @@
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="57">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1671,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1749,7 +1769,7 @@
         <v>139</v>
       </c>
       <c r="B8" s="70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="29" t="s">
         <v>140</v>
@@ -1952,7 +1972,7 @@
         <v>91</v>
       </c>
       <c r="B30" s="70" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>54</v>
@@ -1994,7 +2014,7 @@
         <v>184</v>
       </c>
       <c r="B34" s="70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34" s="25"/>
     </row>
@@ -2049,148 +2069,168 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1 B6 B41:B1048576">
-    <cfRule type="containsText" dxfId="32" priority="634" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="56" priority="646" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="containsText" dxfId="31" priority="632" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="55" priority="644" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="containsText" dxfId="30" priority="631" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="54" priority="643" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="containsText" dxfId="29" priority="630" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="53" priority="642" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="containsText" dxfId="28" priority="629" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="52" priority="641" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39 B17:B18">
-    <cfRule type="containsText" dxfId="27" priority="628" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="51" priority="640" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="containsText" dxfId="26" priority="618" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="50" priority="630" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="25" priority="552" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="49" priority="564" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B11">
-    <cfRule type="containsText" dxfId="24" priority="437" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="48" priority="449" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="containsText" dxfId="23" priority="436" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="47" priority="448" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="containsText" dxfId="22" priority="324" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="46" priority="336" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="containsText" dxfId="21" priority="311" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="45" priority="323" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="20" priority="281" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="44" priority="293" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="19" priority="279" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="43" priority="291" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="18" priority="230" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="42" priority="242" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="containsText" dxfId="17" priority="124" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="41" priority="136" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="containsText" dxfId="16" priority="106" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="40" priority="118" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="15" priority="61" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="39" priority="73" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B37">
+    <cfRule type="containsText" dxfId="36" priority="29" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
+    <cfRule type="containsText" dxfId="34" priority="13" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="containsText" dxfId="33" priority="24" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="containsText" dxfId="32" priority="23" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
+    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="containsText" dxfId="28" priority="15" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="containsText" dxfId="14" priority="46" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B31)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B31">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="containsText" dxfId="13" priority="18" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B33)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
-    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
-    <cfRule type="containsText" dxfId="11" priority="15" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B34">
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B21)))</formula>
+  <conditionalFormatting sqref="B33">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2318,17 +2358,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="26" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2341,8 +2381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2641,11 +2681,11 @@
       <c r="A33" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="B33" s="42">
-        <v>12</v>
+      <c r="B33" s="84">
+        <v>30</v>
       </c>
       <c r="C33" s="58" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2670,7 +2710,7 @@
       <c r="A36" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="B36" s="42">
+      <c r="B36" s="84">
         <v>0.8</v>
       </c>
       <c r="C36" s="58" t="s">
@@ -2681,7 +2721,7 @@
       <c r="A37" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="B37" s="42">
+      <c r="B37" s="84">
         <v>1</v>
       </c>
       <c r="C37" s="58" t="s">
@@ -2736,7 +2776,7 @@
         <v>180</v>
       </c>
       <c r="B43" s="42">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C43" s="58"/>
     </row>
@@ -2778,7 +2818,8 @@
         <v>191</v>
       </c>
       <c r="B48" s="75">
-        <v>12</v>
+        <f>B33</f>
+        <v>30</v>
       </c>
       <c r="C48" s="83" t="s">
         <v>190</v>
@@ -2929,7 +2970,8 @@
         <v>192</v>
       </c>
       <c r="B63" s="44">
-        <v>12</v>
+        <f>B33</f>
+        <v>30</v>
       </c>
       <c r="C63" s="25" t="s">
         <v>190</v>
@@ -3232,7 +3274,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="24" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added ability to email figures as attachments renamed some figures updated settings excel file, added email column in fig_settings tab moved the mean_AAIMON_all_TMDs to gather.py changed the save_figure function save lowres as default for fig with 5 million datapoints
</commit_message>
<xml_diff>
--- a/korbinian/examples/settings/korbinian_run_settings_schweris_mp.xlsx
+++ b/korbinian/examples/settings/korbinian_run_settings_schweris_mp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="3375" windowWidth="14265" windowHeight="7440"/>
+    <workbookView xWindow="3195" yWindow="3435" windowWidth="14265" windowHeight="7380" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="run_settings" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="variables" sheetId="2" r:id="rId3"/>
     <sheet name="figs_settings" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="237">
   <si>
     <t>protein_lists</t>
   </si>
@@ -601,12 +601,6 @@
     <t>run_calc_fastagap_densities</t>
   </si>
   <si>
-    <t>save_fig_to_pdf</t>
-  </si>
-  <si>
-    <t>save_fig_to_png</t>
-  </si>
-  <si>
     <t>Fig01_Histogram_of_mean_AAIMON_and_AASMON_ratios_SP_vs_MP</t>
   </si>
   <si>
@@ -634,9 +628,6 @@
     <t>Fig08_Scattergram_comparing_total_number_of_simap_hits_with_mean_AAIMON</t>
   </si>
   <si>
-    <t>note_that_the_total_hits_comes_from_SIMAP,_so_this_doesn't_say_anything_about_how_much_data_is_available_for_each_protein</t>
-  </si>
-  <si>
     <t>Fig09_Histogram_of_mean_AAIMON_ratios_for_each_TMD_separately</t>
   </si>
   <si>
@@ -674,13 +665,76 @@
   </si>
   <si>
     <t>Fig21_Boxplot_only_GPCRs</t>
+  </si>
+  <si>
+    <t>cutoff_max_characterising_each_homol_TMD</t>
+  </si>
+  <si>
+    <t>cutoff_min_characterising_each_homol_TMD</t>
+  </si>
+  <si>
+    <t>specify_number_of_bins_characterising_TMDs</t>
+  </si>
+  <si>
+    <t>100 is equivalent to one bin every 1% identity</t>
+  </si>
+  <si>
+    <t>save_df_characterising_each_homol_TMD</t>
+  </si>
+  <si>
+    <t>"run_gather_AAIMON_ratios = TRUE" is required!!  AAIMON and AAIMON_n of each TMD and homologue is saved as zipped pickle, a second df is saved containing binned data in 1% identity steps and 95% confidence intervals</t>
+  </si>
+  <si>
+    <t>note_that_the_total_hits_comes_from_SIMAP,_so_this_doesn't_say_anything_about_how_much_data_is_available_for_each_protein; total_hits = n_homol_TM01</t>
+  </si>
+  <si>
+    <t>Fig22_Boxplot_comparing_number_of_TMDs_with_mean_AAIMON</t>
+  </si>
+  <si>
+    <t>Fig23_Boxplot_comparing_seqlen_with_mean_AAIMON</t>
+  </si>
+  <si>
+    <t>Email settings</t>
+  </si>
+  <si>
+    <t>send_email_when_finished</t>
+  </si>
+  <si>
+    <t>send_email_to</t>
+  </si>
+  <si>
+    <t>email_message</t>
+  </si>
+  <si>
+    <t>mark.teese@tum.de</t>
+  </si>
+  <si>
+    <t>Your korbinian run has finished.</t>
+  </si>
+  <si>
+    <t>save_pdf</t>
+  </si>
+  <si>
+    <t>save_png</t>
+  </si>
+  <si>
+    <t>Fig98_Scatterplot_AAIMON_vs_perc_ident_all_homol_all_proteins</t>
+  </si>
+  <si>
+    <t>Fig99_Linegraph_CI_95_AAIMON_vs_perc_ident_all_homol_all_proteins</t>
+  </si>
+  <si>
+    <t>min_n_homol_for_figs</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -711,8 +765,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -863,6 +925,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -873,10 +941,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1068,11 +1137,260 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="67">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1610,10 +1928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF46"/>
+  <dimension ref="A1:AF48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,7 +1993,7 @@
         <v>166</v>
       </c>
       <c r="B3" s="37">
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="C3" s="54" t="s">
         <v>6</v>
@@ -2246,7 +2564,7 @@
         <v>122</v>
       </c>
       <c r="B21" s="70" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>11</v>
@@ -2461,7 +2779,7 @@
         <v>91</v>
       </c>
       <c r="B30" s="70" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>54</v>
@@ -2538,12 +2856,14 @@
     </row>
     <row r="32" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>181</v>
+        <v>220</v>
       </c>
       <c r="B32" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="25"/>
+      <c r="C32" s="25" t="s">
+        <v>221</v>
+      </c>
       <c r="D32" s="62"/>
       <c r="E32" s="62"/>
       <c r="F32" s="62"/>
@@ -2576,7 +2896,7 @@
     </row>
     <row r="33" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="B33" s="70" t="s">
         <v>5</v>
@@ -2613,9 +2933,13 @@
       <c r="AF33" s="62"/>
     </row>
     <row r="34" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="62"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="62"/>
+      <c r="A34" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B34" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="25"/>
       <c r="D34" s="62"/>
       <c r="E34" s="62"/>
       <c r="F34" s="62"/>
@@ -2647,11 +2971,9 @@
       <c r="AF34" s="62"/>
     </row>
     <row r="35" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="45"/>
-      <c r="C35" s="60"/>
+      <c r="A35" s="62"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="62"/>
       <c r="D35" s="62"/>
       <c r="E35" s="62"/>
       <c r="F35" s="62"/>
@@ -2683,15 +3005,11 @@
       <c r="AF35" s="62"/>
     </row>
     <row r="36" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="B36" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="61" t="s">
-        <v>56</v>
-      </c>
+      <c r="A36" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="45"/>
+      <c r="C36" s="60"/>
       <c r="D36" s="62"/>
       <c r="E36" s="62"/>
       <c r="F36" s="62"/>
@@ -2722,15 +3040,15 @@
       <c r="AE36" s="62"/>
       <c r="AF36" s="62"/>
     </row>
-    <row r="37" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B37" s="70" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C37" s="61" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="D37" s="62"/>
       <c r="E37" s="62"/>
@@ -2762,16 +3080,29 @@
       <c r="AE37" s="62"/>
       <c r="AF37" s="62"/>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B38" s="70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38" s="61" t="s">
-        <v>15</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="62"/>
+      <c r="K38" s="62"/>
+      <c r="L38" s="62"/>
+      <c r="M38" s="62"/>
+      <c r="N38" s="62"/>
+      <c r="O38" s="62"/>
+      <c r="P38" s="62"/>
       <c r="Q38" s="62"/>
       <c r="R38" s="62"/>
       <c r="S38" s="62"/>
@@ -2790,8 +3121,15 @@
       <c r="AF38" s="62"/>
     </row>
     <row r="39" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A39" s="62"/>
-      <c r="C39" s="62"/>
+      <c r="A39" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="61" t="s">
+        <v>15</v>
+      </c>
       <c r="Q39" s="62"/>
       <c r="R39" s="62"/>
       <c r="S39" s="62"/>
@@ -2809,29 +3147,9 @@
       <c r="AE39" s="62"/>
       <c r="AF39" s="62"/>
     </row>
-    <row r="40" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="85" t="s">
-        <v>92</v>
-      </c>
-      <c r="B40" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="86" t="s">
-        <v>55</v>
-      </c>
-      <c r="D40" s="62"/>
-      <c r="E40" s="62"/>
-      <c r="F40" s="62"/>
-      <c r="G40" s="62"/>
-      <c r="H40" s="62"/>
-      <c r="I40" s="62"/>
-      <c r="J40" s="62"/>
-      <c r="K40" s="62"/>
-      <c r="L40" s="62"/>
-      <c r="M40" s="62"/>
-      <c r="N40" s="62"/>
-      <c r="O40" s="62"/>
-      <c r="P40" s="62"/>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A40" s="62"/>
+      <c r="C40" s="62"/>
       <c r="Q40" s="62"/>
       <c r="R40" s="62"/>
       <c r="S40" s="62"/>
@@ -2851,12 +3169,14 @@
     </row>
     <row r="41" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="85" t="s">
-        <v>176</v>
+        <v>92</v>
       </c>
       <c r="B41" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="86"/>
+      <c r="C41" s="86" t="s">
+        <v>55</v>
+      </c>
       <c r="D41" s="62"/>
       <c r="E41" s="62"/>
       <c r="F41" s="62"/>
@@ -2887,14 +3207,27 @@
       <c r="AE41" s="62"/>
       <c r="AF41" s="62"/>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>93</v>
+    <row r="42" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="85" t="s">
+        <v>176</v>
       </c>
       <c r="B42" s="70" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="86"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="62"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="62"/>
+      <c r="N42" s="62"/>
+      <c r="O42" s="62"/>
+      <c r="P42" s="62"/>
       <c r="Q42" s="62"/>
       <c r="R42" s="62"/>
       <c r="S42" s="62"/>
@@ -2913,6 +3246,13 @@
       <c r="AF42" s="62"/>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="86"/>
       <c r="Q43" s="62"/>
       <c r="R43" s="62"/>
       <c r="S43" s="62"/>
@@ -2948,7 +3288,25 @@
       <c r="AE44" s="62"/>
       <c r="AF44" s="62"/>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="B45" s="90"/>
+      <c r="C45" s="91"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="62"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="62"/>
+      <c r="L45" s="62"/>
+      <c r="M45" s="62"/>
+      <c r="N45" s="62"/>
+      <c r="O45" s="62"/>
+      <c r="P45" s="62"/>
       <c r="Q45" s="62"/>
       <c r="R45" s="62"/>
       <c r="S45" s="62"/>
@@ -2967,6 +3325,12 @@
       <c r="AF45" s="62"/>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A46" s="62" t="s">
+        <v>226</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="Q46" s="62"/>
       <c r="R46" s="62"/>
       <c r="S46" s="62"/>
@@ -2984,129 +3348,195 @@
       <c r="AE46" s="62"/>
       <c r="AF46" s="62"/>
     </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A47" s="62" t="s">
+        <v>227</v>
+      </c>
+      <c r="B47" s="92" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q47" s="62"/>
+      <c r="R47" s="62"/>
+      <c r="S47" s="62"/>
+      <c r="T47" s="62"/>
+      <c r="U47" s="62"/>
+      <c r="V47" s="62"/>
+      <c r="W47" s="62"/>
+      <c r="X47" s="62"/>
+      <c r="Y47" s="62"/>
+      <c r="Z47" s="62"/>
+      <c r="AA47" s="62"/>
+      <c r="AB47" s="62"/>
+      <c r="AC47" s="62"/>
+      <c r="AD47" s="62"/>
+      <c r="AE47" s="62"/>
+      <c r="AF47" s="62"/>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A48" s="62" t="s">
+        <v>228</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q48" s="62"/>
+      <c r="R48" s="62"/>
+      <c r="S48" s="62"/>
+      <c r="T48" s="62"/>
+      <c r="U48" s="62"/>
+      <c r="V48" s="62"/>
+      <c r="W48" s="62"/>
+      <c r="X48" s="62"/>
+      <c r="Y48" s="62"/>
+      <c r="Z48" s="62"/>
+      <c r="AA48" s="62"/>
+      <c r="AB48" s="62"/>
+      <c r="AC48" s="62"/>
+      <c r="AD48" s="62"/>
+      <c r="AE48" s="62"/>
+      <c r="AF48" s="62"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B6 B43:B1048576">
-    <cfRule type="containsText" dxfId="32" priority="733" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="B1 B6 B44 B49:B1048576">
+    <cfRule type="containsText" dxfId="60" priority="766" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="containsText" dxfId="31" priority="731" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="59" priority="764" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="containsText" dxfId="30" priority="730" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="58" priority="763" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B26)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B34">
-    <cfRule type="containsText" dxfId="29" priority="729" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B34)))</formula>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="containsText" dxfId="57" priority="762" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B35)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
-    <cfRule type="containsText" dxfId="28" priority="728" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B39)))</formula>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="containsText" dxfId="56" priority="761" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B40)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38 B17:B18">
-    <cfRule type="containsText" dxfId="27" priority="727" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="B39 B17:B18">
+    <cfRule type="containsText" dxfId="55" priority="760" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:B20">
-    <cfRule type="containsText" dxfId="26" priority="651" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="54" priority="684" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B11">
-    <cfRule type="containsText" dxfId="25" priority="536" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="53" priority="569" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="containsText" dxfId="24" priority="535" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="52" priority="568" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="containsText" dxfId="23" priority="423" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="51" priority="456" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="22" priority="378" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="50" priority="411" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="21" priority="329" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="49" priority="362" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="containsText" dxfId="20" priority="223" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="48" priority="256" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B24)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
-    <cfRule type="containsText" dxfId="19" priority="116" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B36)))</formula>
+  <conditionalFormatting sqref="B37">
+    <cfRule type="containsText" dxfId="47" priority="149" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="containsText" dxfId="18" priority="43" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="46" priority="76" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="45" priority="46" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B14)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B40:B42">
-    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B30)))</formula>
+  <conditionalFormatting sqref="B41:B43">
+    <cfRule type="containsText" dxfId="44" priority="42" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="43" priority="39" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B29">
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="42" priority="38" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:B33">
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="B34">
+    <cfRule type="containsText" dxfId="41" priority="37" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33">
+    <cfRule type="containsText" dxfId="39" priority="33" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="containsText" dxfId="35" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B32)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B38">
+    <cfRule type="containsText" dxfId="34" priority="7" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="containsText" dxfId="31" priority="9" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="containsText" dxfId="27" priority="5" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46:B48">
+    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B31)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B47" r:id="rId1" display="martin.ortner@tum.de"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3227,17 +3657,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3248,10 +3678,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4010,140 +4440,169 @@
       </c>
       <c r="C82" s="61"/>
     </row>
-    <row r="84" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="26" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="B83" s="46">
+        <v>4500</v>
+      </c>
+      <c r="C83" s="61"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="B84" s="46">
+        <v>50</v>
+      </c>
+      <c r="C84" s="61"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="B85" s="46">
+        <v>100</v>
+      </c>
+      <c r="C85" s="61" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B84" s="48"/>
-      <c r="C84" s="27"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B85" s="49">
-        <v>0</v>
-      </c>
-      <c r="C85" s="29"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B86" s="49">
-        <v>-12</v>
-      </c>
-      <c r="C86" s="29"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B87" s="49">
-        <v>-2</v>
-      </c>
-      <c r="C87" s="29"/>
+      <c r="B87" s="48"/>
+      <c r="C87" s="27"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B88" s="49" t="s">
-        <v>40</v>
+        <v>32</v>
+      </c>
+      <c r="B88" s="49">
+        <v>0</v>
       </c>
       <c r="C88" s="29"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="28" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B89" s="49">
-        <v>-0.2</v>
+        <v>-12</v>
       </c>
       <c r="C89" s="29"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="28" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B90" s="49">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="C90" s="29"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B91" s="49">
-        <v>-1</v>
+        <v>35</v>
+      </c>
+      <c r="B91" s="49" t="s">
+        <v>40</v>
       </c>
       <c r="C91" s="29"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="28" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B92" s="49">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="C92" s="29"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B93" s="49">
+        <v>-1</v>
+      </c>
+      <c r="C93" s="29"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B94" s="49">
+        <v>-1</v>
+      </c>
+      <c r="C94" s="29"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B95" s="49">
+        <v>0</v>
+      </c>
+      <c r="C95" s="29"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B93" s="49" t="s">
+      <c r="B96" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="C93" s="29"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="34" t="s">
+      <c r="C96" s="29"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B95" s="50"/>
-      <c r="C95" s="30"/>
-    </row>
-    <row r="96" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="11" t="s">
+      <c r="B98" s="50"/>
+      <c r="C98" s="30"/>
+    </row>
+    <row r="99" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B96" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="C96" s="33"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="11" t="s">
+      <c r="B99" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" s="33"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B97" s="51">
-        <v>5</v>
-      </c>
-      <c r="C97" s="33"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="11" t="s">
+      <c r="B100" s="51">
+        <v>5</v>
+      </c>
+      <c r="C100" s="33"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B98" s="51" t="s">
+      <c r="B101" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C98" s="33"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="11" t="s">
+      <c r="C101" s="33"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B99" s="51" t="s">
+      <c r="B102" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C99" s="51"/>
+      <c r="C102" s="51"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4154,239 +4613,417 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.5703125" customWidth="1"/>
+    <col min="1" max="1" width="77.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>96</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="88" t="s">
-        <v>194</v>
+        <v>231</v>
       </c>
       <c r="B2" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="87"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="70"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="87"/>
+      <c r="P2" s="87"/>
+      <c r="Q2" s="87"/>
+    </row>
+    <row r="3" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="88" t="s">
-        <v>195</v>
+        <v>232</v>
       </c>
       <c r="B3" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="87"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>196</v>
-      </c>
-      <c r="B4" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="70"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
+      <c r="Q3" s="87"/>
+    </row>
+    <row r="4" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="88" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4" s="70">
+        <v>50</v>
+      </c>
+      <c r="C4" s="70"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="87"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B5" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="70" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B8" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>199</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B9" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>201</v>
+      </c>
+      <c r="B11" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>204</v>
+      </c>
+      <c r="B14" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>205</v>
+      </c>
+      <c r="B15" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>207</v>
+      </c>
+      <c r="B17" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>208</v>
+      </c>
+      <c r="B18" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>209</v>
+      </c>
+      <c r="B19" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>211</v>
+      </c>
+      <c r="B21" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>212</v>
+      </c>
+      <c r="B22" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>213</v>
+      </c>
+      <c r="B23" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>214</v>
+      </c>
+      <c r="B24" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>215</v>
+      </c>
+      <c r="B25" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>223</v>
+      </c>
+      <c r="B26" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>224</v>
+      </c>
+      <c r="B27" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>233</v>
+      </c>
+      <c r="B28" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>234</v>
+      </c>
+      <c r="B29" s="70" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B7" s="70" t="s">
+      <c r="C29" s="70" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>201</v>
-      </c>
-      <c r="B8" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>202</v>
-      </c>
-      <c r="B9" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>203</v>
-      </c>
-      <c r="B10" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>204</v>
-      </c>
-      <c r="B11" s="70" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>206</v>
-      </c>
-      <c r="B12" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>207</v>
-      </c>
-      <c r="B13" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>208</v>
-      </c>
-      <c r="B14" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>209</v>
-      </c>
-      <c r="B15" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>210</v>
-      </c>
-      <c r="B16" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>211</v>
-      </c>
-      <c r="B17" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>212</v>
-      </c>
-      <c r="B18" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>213</v>
-      </c>
-      <c r="B19" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>214</v>
-      </c>
-      <c r="B20" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>215</v>
-      </c>
-      <c r="B21" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>216</v>
-      </c>
-      <c r="B22" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>217</v>
-      </c>
-      <c r="B23" s="70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>218</v>
-      </c>
-      <c r="B24" s="70" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="B1:C1">
+    <cfRule type="containsText" dxfId="19" priority="14" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:B23">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B4)))</formula>
+  <conditionalFormatting sqref="B2:C4">
+    <cfRule type="containsText" dxfId="18" priority="10" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B24)))</formula>
+  <conditionalFormatting sqref="B5:C5">
+    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
+  <conditionalFormatting sqref="B6:C27">
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28:C28">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
IMPORTANT. Massive change to settings file. Best to copy from MT.  - shortened run names  - removed list_number from 100 places in code, and replaced with s["list_number"]  - fixed bugs in filtering of prot_lists  - added backup of settings file  - added comments and refactored "run_korbinian", using single or mult lists
</commit_message>
<xml_diff>
--- a/korbinian/examples/settings/korbinian_run_settings_schweris_mp.xlsx
+++ b/korbinian/examples/settings/korbinian_run_settings_schweris_mp.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="585" windowWidth="25605" windowHeight="14535"/>
+    <workbookView xWindow="0" yWindow="645" windowWidth="25605" windowHeight="14475"/>
   </bookViews>
   <sheets>
-    <sheet name="run_settings" sheetId="1" r:id="rId1"/>
-    <sheet name="file_locations" sheetId="3" r:id="rId2"/>
+    <sheet name="run" sheetId="1" r:id="rId1"/>
+    <sheet name="files" sheetId="3" r:id="rId2"/>
     <sheet name="variables" sheetId="2" r:id="rId3"/>
-    <sheet name="figs_settings" sheetId="4" r:id="rId4"/>
+    <sheet name="figs" sheetId="4" r:id="rId4"/>
+    <sheet name="lists" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="243">
   <si>
     <t>protein_lists</t>
   </si>
@@ -69,9 +70,6 @@
     <t>If "TRUE", figures will be created describing the AAIMON ratios (and other variables) of the list of proteins.</t>
   </si>
   <si>
-    <t>If "TRUE", two or more protein lists will be compared (e.g. single-pass vs multi-pass), and a number of figures created and saved.</t>
-  </si>
-  <si>
     <t>uniref_cluster_cutoff</t>
   </si>
   <si>
@@ -87,9 +85,6 @@
     <t>overwrite_csv_file_av_cons_ratios_hits</t>
   </si>
   <si>
-    <t>["patent","Patent","synthetic","Synthetic","artificial","Artificial","bad sequence","low quality"]</t>
-  </si>
-  <si>
     <t>gap_open_penalty_min</t>
   </si>
   <si>
@@ -177,9 +172,6 @@
     <t xml:space="preserve">Java Executable String (usually "java", or %JAVAJRE%, depending on java_home settings in Windows). </t>
   </si>
   <si>
-    <t>UniProt non-redundancy parameters</t>
-  </si>
-  <si>
     <t>SIMAP homologue download parameters</t>
   </si>
   <si>
@@ -240,33 +232,6 @@
     <t>Analysis run settings</t>
   </si>
   <si>
-    <t>run_parse_large_flatfile_with_list_uniprot_accessions</t>
-  </si>
-  <si>
-    <t>run_retrieve_uniprot_data_for_acc_list_in_xlsx_file</t>
-  </si>
-  <si>
-    <t>run_create_csv_from_uniprot_flatfile</t>
-  </si>
-  <si>
-    <t>run_parse_simap_to_csv</t>
-  </si>
-  <si>
-    <t>run_calculate_AAIMON_ratios</t>
-  </si>
-  <si>
-    <t>run_calculate_gap_densities</t>
-  </si>
-  <si>
-    <t>run_create_graph_of_gap_density</t>
-  </si>
-  <si>
-    <t>run_save_figures_describing_proteins_in_list</t>
-  </si>
-  <si>
-    <t>run_compare_lists</t>
-  </si>
-  <si>
     <t>parameter</t>
   </si>
   <si>
@@ -342,12 +307,6 @@
     <t>do you want redundant selected (e.g. TMD) sequences to be removed before saving to fasta</t>
   </si>
   <si>
-    <t>run_setup_df_file_locations</t>
-  </si>
-  <si>
-    <t>run_create_fasta</t>
-  </si>
-  <si>
     <t>slice_juxtamembrane_regions</t>
   </si>
   <si>
@@ -423,9 +382,6 @@
     <t>Number of amino acids after the TMD, for slicing "TMD_plus_surr" sequence.</t>
   </si>
   <si>
-    <t>homologue parsing and slicing settings</t>
-  </si>
-  <si>
     <t>cr_min_identity_of_full_protein</t>
   </si>
   <si>
@@ -435,9 +391,6 @@
     <t>Mark Teese</t>
   </si>
   <si>
-    <t>run_gather_AAIMON_ratios</t>
-  </si>
-  <si>
     <t>overwrite_simap_parsed_to_csv</t>
   </si>
   <si>
@@ -468,9 +421,6 @@
     <t>D:\Databases\simap</t>
   </si>
   <si>
-    <t>run_download_homologues</t>
-  </si>
-  <si>
     <t>OMPdb_get_TM_indices_and_slice</t>
   </si>
   <si>
@@ -483,9 +433,6 @@
     <t>Only for comparing two or more protein lists. Here you can name the protein lists that you are analysing.</t>
   </si>
   <si>
-    <t>run_slice_TMDs_from_homologues</t>
-  </si>
-  <si>
     <t>Number of concurrent processes to be run, using multiple CPU cores if available.</t>
   </si>
   <si>
@@ -504,9 +451,6 @@
     <t>gap_allowed_gaps_per_tmd</t>
   </si>
   <si>
-    <t>run_gather_gap_densities</t>
-  </si>
-  <si>
     <t>fa_max_n_gaps_in_match_TMD_plus_surr</t>
   </si>
   <si>
@@ -519,9 +463,6 @@
     <t>fa_min_n_gaps_in_match_TMD_plus_surr</t>
   </si>
   <si>
-    <t>run_fastagap_save</t>
-  </si>
-  <si>
     <t>cr_max_n_gaps_in_TMD</t>
   </si>
   <si>
@@ -555,9 +496,6 @@
     <t>D:\Databases\programs\clustal-omega\clustalo.exe</t>
   </si>
   <si>
-    <t>run_calc_fastagap_densities</t>
-  </si>
-  <si>
     <t>Fig01_Histogram_of_mean_AAIMON_and_AASMON_ratios_SP_vs_MP</t>
   </si>
   <si>
@@ -687,9 +625,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>run_filter_truncated_alignments</t>
-  </si>
-  <si>
     <t>run_keyword_analysis</t>
   </si>
   <si>
@@ -733,6 +668,90 @@
   </si>
   <si>
     <t>Special analysis settings</t>
+  </si>
+  <si>
+    <t>["patent","synthetic","artificial","bad sequence","low quality"]</t>
+  </si>
+  <si>
+    <t>Protein list non-redundancy parameters</t>
+  </si>
+  <si>
+    <t>Homologue parsing and slicing settings</t>
+  </si>
+  <si>
+    <t>OMPdb_topology_reliability_cutoff</t>
+  </si>
+  <si>
+    <t>gather_pretty_alignments</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>max_lipo_list</t>
+  </si>
+  <si>
+    <t>max_lipo_homol</t>
+  </si>
+  <si>
+    <t>min_homol</t>
+  </si>
+  <si>
+    <t>rand_TM</t>
+  </si>
+  <si>
+    <t>rand_nonTM</t>
+  </si>
+  <si>
+    <t>prepare_protein_list</t>
+  </si>
+  <si>
+    <t>download_homologues</t>
+  </si>
+  <si>
+    <t>parse_large_flatfile_with_list_uniprot_accessions</t>
+  </si>
+  <si>
+    <t>retrieve_uniprot_data_for_acc_list_in_xlsx_file</t>
+  </si>
+  <si>
+    <t>create_csv_from_uniprot_flatfile</t>
+  </si>
+  <si>
+    <t>parse_simap_to_csv</t>
+  </si>
+  <si>
+    <t>slice_TMDs_from_homologues</t>
+  </si>
+  <si>
+    <t>calculate_AAIMON_ratios</t>
+  </si>
+  <si>
+    <t>gather_AAIMON_ratios</t>
+  </si>
+  <si>
+    <t>save_figures_describing_proteins_in_list</t>
+  </si>
+  <si>
+    <t>filter_truncated_alignments</t>
+  </si>
+  <si>
+    <t>create_fasta</t>
+  </si>
+  <si>
+    <t>save_fastagap</t>
+  </si>
+  <si>
+    <t>calc_fastagap_densities</t>
+  </si>
+  <si>
+    <t>create_graph_of_gap_density</t>
+  </si>
+  <si>
+    <t>calculate_gap_densities</t>
+  </si>
+  <si>
+    <t>gather_gap_densities</t>
   </si>
 </sst>
 </file>
@@ -1853,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B28" activeCellId="3" sqref="B20:B21 B24:B25 B25 B28:B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1869,13 +1888,13 @@
   <sheetData>
     <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D1" s="84"/>
       <c r="E1" s="84"/>
@@ -1893,7 +1912,7 @@
     </row>
     <row r="2" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B2" s="35"/>
       <c r="C2" s="52"/>
@@ -1913,10 +1932,10 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B3" s="36">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C3" s="53" t="s">
         <v>6</v>
@@ -1946,7 +1965,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="Q4" s="61"/>
       <c r="R4" s="61"/>
@@ -1973,7 +1992,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="Q5" s="61"/>
       <c r="R5" s="61"/>
@@ -1997,7 +2016,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B7" s="47"/>
       <c r="C7" s="26"/>
@@ -2020,13 +2039,13 @@
     </row>
     <row r="8" spans="1:32" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B8" s="69" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="D8" s="61"/>
       <c r="E8" s="61"/>
@@ -2060,13 +2079,13 @@
     </row>
     <row r="9" spans="1:32" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="B9" s="69">
         <v>14</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="D9" s="61"/>
       <c r="E9" s="61"/>
@@ -2100,13 +2119,13 @@
     </row>
     <row r="10" spans="1:32" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B10" s="69" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="D10" s="61"/>
       <c r="E10" s="61"/>
@@ -2140,13 +2159,13 @@
     </row>
     <row r="11" spans="1:32" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B11" s="69" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="D11" s="61"/>
       <c r="E11" s="61"/>
@@ -2200,7 +2219,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B13" s="38"/>
       <c r="C13" s="54"/>
@@ -2223,7 +2242,7 @@
     </row>
     <row r="14" spans="1:32" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="B14" s="69" t="s">
         <v>5</v>
@@ -2261,7 +2280,7 @@
     </row>
     <row r="15" spans="1:32" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B15" s="69" t="s">
         <v>5</v>
@@ -2299,13 +2318,13 @@
     </row>
     <row r="16" spans="1:32" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="B16" s="69" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
       <c r="D16" s="61"/>
       <c r="E16" s="61"/>
@@ -2339,7 +2358,7 @@
     </row>
     <row r="17" spans="1:32" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>72</v>
+        <v>228</v>
       </c>
       <c r="B17" s="69" t="s">
         <v>5</v>
@@ -2379,7 +2398,7 @@
     </row>
     <row r="18" spans="1:32" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>73</v>
+        <v>229</v>
       </c>
       <c r="B18" s="69" t="s">
         <v>5</v>
@@ -2419,7 +2438,7 @@
     </row>
     <row r="19" spans="1:32" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B19" s="69" t="s">
         <v>5</v>
@@ -2459,7 +2478,7 @@
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>74</v>
+        <v>230</v>
       </c>
       <c r="B20" s="69" t="s">
         <v>5</v>
@@ -2486,10 +2505,10 @@
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>106</v>
+        <v>226</v>
       </c>
       <c r="B21" s="69" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="31" t="s">
         <v>11</v>
@@ -2533,7 +2552,7 @@
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B23" s="40"/>
       <c r="C23" s="56"/>
@@ -2556,7 +2575,7 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="63" t="s">
-        <v>148</v>
+        <v>227</v>
       </c>
       <c r="B24" s="69" t="s">
         <v>5</v>
@@ -2583,7 +2602,7 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="65" t="s">
-        <v>75</v>
+        <v>231</v>
       </c>
       <c r="B25" s="69" t="s">
         <v>5</v>
@@ -2614,20 +2633,20 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B27" s="42"/>
       <c r="C27" s="58"/>
     </row>
     <row r="28" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>153</v>
+        <v>232</v>
       </c>
       <c r="B28" s="69" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="D28" s="61"/>
       <c r="E28" s="61"/>
@@ -2661,13 +2680,13 @@
     </row>
     <row r="29" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>76</v>
+        <v>233</v>
       </c>
       <c r="B29" s="69" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D29" s="61"/>
       <c r="E29" s="61"/>
@@ -2701,13 +2720,13 @@
     </row>
     <row r="30" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>137</v>
+        <v>234</v>
       </c>
       <c r="B30" s="69" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D30" s="61"/>
       <c r="E30" s="61"/>
@@ -2741,13 +2760,13 @@
     </row>
     <row r="31" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="B31" s="69" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="D31" s="61"/>
       <c r="E31" s="61"/>
@@ -2781,7 +2800,7 @@
     </row>
     <row r="32" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="B32" s="69" t="s">
         <v>5</v>
@@ -2819,10 +2838,10 @@
     </row>
     <row r="33" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>79</v>
+        <v>235</v>
       </c>
       <c r="B33" s="69" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C33" s="24" t="s">
         <v>14</v>
@@ -2893,7 +2912,7 @@
     </row>
     <row r="35" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>236</v>
+        <v>214</v>
       </c>
       <c r="B35" s="44"/>
       <c r="C35" s="59"/>
@@ -2929,7 +2948,7 @@
     </row>
     <row r="36" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="B36" s="69" t="s">
         <v>5</v>
@@ -2967,14 +2986,12 @@
     </row>
     <row r="37" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
-        <v>107</v>
+        <v>219</v>
       </c>
       <c r="B37" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="60" t="s">
-        <v>43</v>
-      </c>
+      <c r="C37" s="60"/>
       <c r="D37" s="61"/>
       <c r="E37" s="61"/>
       <c r="F37" s="61"/>
@@ -3007,12 +3024,14 @@
     </row>
     <row r="38" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
-        <v>165</v>
+        <v>237</v>
       </c>
       <c r="B38" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="60"/>
+      <c r="C38" s="60" t="s">
+        <v>41</v>
+      </c>
       <c r="D38" s="61"/>
       <c r="E38" s="61"/>
       <c r="F38" s="61"/>
@@ -3045,7 +3064,7 @@
     </row>
     <row r="39" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>177</v>
+        <v>238</v>
       </c>
       <c r="B39" s="69" t="s">
         <v>5</v>
@@ -3083,14 +3102,12 @@
     </row>
     <row r="40" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
-        <v>78</v>
+        <v>239</v>
       </c>
       <c r="B40" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="60" t="s">
-        <v>45</v>
-      </c>
+      <c r="C40" s="60"/>
       <c r="D40" s="61"/>
       <c r="E40" s="61"/>
       <c r="F40" s="61"/>
@@ -3123,13 +3140,13 @@
     </row>
     <row r="41" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
-        <v>77</v>
+        <v>240</v>
       </c>
       <c r="B41" s="69" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="60" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D41" s="61"/>
       <c r="E41" s="61"/>
@@ -3163,12 +3180,14 @@
     </row>
     <row r="42" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
-        <v>160</v>
+        <v>241</v>
       </c>
       <c r="B42" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="60"/>
+      <c r="C42" s="60" t="s">
+        <v>42</v>
+      </c>
       <c r="D42" s="61"/>
       <c r="E42" s="61"/>
       <c r="F42" s="61"/>
@@ -3199,14 +3218,27 @@
       <c r="AE42" s="61"/>
       <c r="AF42" s="61"/>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>78</v>
+        <v>242</v>
       </c>
       <c r="B43" s="69" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="60"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="61"/>
+      <c r="G43" s="61"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="61"/>
+      <c r="J43" s="61"/>
+      <c r="K43" s="61"/>
+      <c r="L43" s="61"/>
+      <c r="M43" s="61"/>
+      <c r="N43" s="61"/>
+      <c r="O43" s="61"/>
+      <c r="P43" s="61"/>
       <c r="Q43" s="61"/>
       <c r="R43" s="61"/>
       <c r="S43" s="61"/>
@@ -3226,14 +3258,12 @@
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
-        <v>80</v>
+        <v>240</v>
       </c>
       <c r="B44" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="60" t="s">
-        <v>15</v>
-      </c>
+      <c r="C44" s="60"/>
       <c r="Q44" s="61"/>
       <c r="R44" s="61"/>
       <c r="S44" s="61"/>
@@ -3271,7 +3301,7 @@
     </row>
     <row r="46" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="86" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="B46" s="87"/>
       <c r="C46" s="88"/>
@@ -3307,7 +3337,7 @@
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" s="61" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="B47" s="69" t="s">
         <v>5</v>
@@ -3331,10 +3361,10 @@
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A48" s="61" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="B48" s="89" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="Q48" s="61"/>
       <c r="R48" s="61"/>
@@ -3355,10 +3385,10 @@
     </row>
     <row r="49" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A49" s="61" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="Q49" s="61"/>
       <c r="R49" s="61"/>
@@ -3378,92 +3408,112 @@
       <c r="AF49" s="61"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B6 B50:B1048576 B33 B37:B45">
-    <cfRule type="containsText" dxfId="40" priority="895" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="B1 B6 B50:B1048576 B38:B45">
+    <cfRule type="containsText" dxfId="56" priority="979" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="containsText" dxfId="39" priority="893" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="55" priority="977" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="containsText" dxfId="38" priority="892" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="54" priority="976" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="containsText" dxfId="37" priority="891" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="53" priority="975" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B34)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44 B17:B18">
-    <cfRule type="containsText" dxfId="36" priority="889" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="B17:B18">
+    <cfRule type="containsText" dxfId="52" priority="973" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B11">
-    <cfRule type="containsText" dxfId="35" priority="698" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="51" priority="782" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="containsText" dxfId="34" priority="697" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="50" priority="781" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="containsText" dxfId="33" priority="585" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="49" priority="669" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
-    <cfRule type="containsText" dxfId="32" priority="205" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="31" priority="175" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="48" priority="259" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B14)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B41:B43">
-    <cfRule type="containsText" dxfId="30" priority="171" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B41)))</formula>
+  <conditionalFormatting sqref="B42:B44">
+    <cfRule type="containsText" dxfId="47" priority="255" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:B49">
-    <cfRule type="containsText" dxfId="29" priority="133" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="46" priority="217" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="28" priority="103" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="45" priority="187" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="containsText" dxfId="43" priority="64" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47">
+    <cfRule type="containsText" dxfId="42" priority="47" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="27" priority="44" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="41" priority="45" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47">
-    <cfRule type="containsText" dxfId="26" priority="10" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="24" priority="14" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="40" priority="33" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="31" priority="12" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B36)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28:B32 B24:B25 B20:B21">
+  <conditionalFormatting sqref="B21">
+    <cfRule type="containsText" dxfId="29" priority="8" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:B25">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28:B33">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B20)))</formula>
     </cfRule>
@@ -3493,117 +3543,117 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="54"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B10" s="69" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="B11" s="69" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3614,10 +3664,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3629,72 +3679,72 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>51</v>
+        <v>216</v>
       </c>
       <c r="B2" s="35"/>
       <c r="C2" s="52"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="36">
         <v>50</v>
       </c>
       <c r="C3" s="53"/>
     </row>
-    <row r="4" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="54"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" s="36">
+        <v>85</v>
+      </c>
+      <c r="C4" s="53"/>
+    </row>
+    <row r="5" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="37"/>
+      <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="55"/>
+      <c r="A6" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="54"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="55"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>145</v>
+        <v>18</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="55"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>18</v>
+        <v>129</v>
       </c>
       <c r="B9" s="39" t="s">
         <v>5</v>
@@ -3703,87 +3753,87 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="39">
-        <v>2000</v>
-      </c>
-      <c r="C10" s="55" t="s">
-        <v>42</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="55"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" s="39">
-        <v>5000</v>
-      </c>
-      <c r="C11" s="55"/>
+        <v>2000</v>
+      </c>
+      <c r="C11" s="55" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B12" s="39">
-        <v>3000</v>
-      </c>
-      <c r="C12" s="55" t="s">
-        <v>234</v>
-      </c>
+        <v>5000</v>
+      </c>
+      <c r="C12" s="55"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>5</v>
+        <v>32</v>
+      </c>
+      <c r="B13" s="39">
+        <v>3000</v>
       </c>
       <c r="C13" s="55" t="s">
-        <v>118</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="55"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>235</v>
+        <v>34</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C15" s="55"/>
     </row>
-    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="37"/>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="75" t="s">
-        <v>133</v>
-      </c>
-      <c r="B17" s="76"/>
-      <c r="C17" s="77"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="55"/>
+    </row>
+    <row r="17" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="37"/>
+      <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="78" t="s">
-        <v>138</v>
-      </c>
-      <c r="B18" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="80"/>
+      <c r="A18" s="75" t="s">
+        <v>217</v>
+      </c>
+      <c r="B18" s="76"/>
+      <c r="C18" s="77"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="78" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B19" s="79" t="s">
         <v>4</v>
@@ -3792,120 +3842,120 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="78" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20" s="81" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="79" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="80"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="78" t="s">
-        <v>128</v>
-      </c>
-      <c r="B21" s="79" t="s">
-        <v>21</v>
+        <v>94</v>
+      </c>
+      <c r="B21" s="81" t="s">
+        <v>4</v>
       </c>
       <c r="C21" s="80"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="78" t="s">
-        <v>129</v>
-      </c>
-      <c r="B22" s="79">
-        <v>30</v>
-      </c>
-      <c r="C22" s="80" t="s">
-        <v>131</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B22" s="79" t="s">
+        <v>215</v>
+      </c>
+      <c r="C22" s="80"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="78" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="B23" s="79">
         <v>30</v>
       </c>
       <c r="C23" s="80" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="78" t="s">
-        <v>139</v>
-      </c>
-      <c r="B24" s="79" t="b">
+        <v>116</v>
+      </c>
+      <c r="B24" s="79">
+        <v>30</v>
+      </c>
+      <c r="C24" s="80" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="78" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="79" t="b">
         <v>0</v>
       </c>
-      <c r="C24" s="80"/>
-    </row>
-    <row r="25" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="37"/>
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="56"/>
+      <c r="C25" s="80"/>
+    </row>
+    <row r="26" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="37"/>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="B27" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="57" t="s">
-        <v>104</v>
-      </c>
+      <c r="A27" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="40"/>
+      <c r="C27" s="56"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B28" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="57" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B29" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="57" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="B30" s="83">
-        <v>30</v>
+        <v>84</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>4</v>
       </c>
       <c r="C30" s="57" t="s">
-        <v>174</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B31" s="41">
-        <v>2</v>
-      </c>
-      <c r="C31" s="57"/>
+        <v>150</v>
+      </c>
+      <c r="B31" s="83">
+        <v>0.5</v>
+      </c>
+      <c r="C31" s="57" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B32" s="41">
         <v>2</v>
@@ -3914,38 +3964,38 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="83">
-        <v>0.4</v>
-      </c>
-      <c r="C33" s="57" t="s">
-        <v>102</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B33" s="41">
+        <v>2</v>
+      </c>
+      <c r="C33" s="57"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="83">
+        <v>0.4</v>
+      </c>
+      <c r="C34" s="57" t="s">
         <v>90</v>
-      </c>
-      <c r="B34" s="83">
-        <v>1</v>
-      </c>
-      <c r="C34" s="57" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="B35" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="57"/>
+        <v>78</v>
+      </c>
+      <c r="B35" s="83">
+        <v>1</v>
+      </c>
+      <c r="C35" s="57" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B36" s="41" t="s">
         <v>5</v>
@@ -3953,526 +4003,526 @@
       <c r="C36" s="57"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="B37" s="40"/>
-      <c r="C37" s="56"/>
+      <c r="A37" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="57"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="B38" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="57"/>
+      <c r="A38" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B38" s="40"/>
+      <c r="C38" s="56"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="B39" s="41">
-        <v>1</v>
+        <v>144</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>4</v>
       </c>
       <c r="C39" s="57"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="B40" s="41">
+        <v>1</v>
+      </c>
+      <c r="C40" s="57"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" s="41">
         <v>6</v>
       </c>
-      <c r="C40" s="57"/>
-    </row>
-    <row r="41" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="37"/>
-      <c r="C41" s="8"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="70" t="s">
-        <v>98</v>
-      </c>
-      <c r="B42" s="71"/>
-      <c r="C42" s="72"/>
+      <c r="C41" s="57"/>
+    </row>
+    <row r="42" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="37"/>
+      <c r="C42" s="8"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="73" t="s">
-        <v>17</v>
-      </c>
-      <c r="B43" s="74" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="74" t="s">
-        <v>4</v>
-      </c>
+      <c r="A43" s="70" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="71"/>
+      <c r="C43" s="72"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="B44" s="74">
-        <v>2</v>
-      </c>
-      <c r="C44" s="74">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="B44" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="74" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="73" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="B45" s="74">
-        <f>B30</f>
-        <v>30</v>
-      </c>
-      <c r="C45" s="82" t="s">
-        <v>171</v>
+        <v>2</v>
+      </c>
+      <c r="C45" s="74">
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="73" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="B46" s="74">
-        <f>B33</f>
-        <v>0.4</v>
+        <f>B31</f>
+        <v>0.5</v>
       </c>
       <c r="C46" s="82" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="73" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="B47" s="74">
         <f>B34</f>
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="C47" s="82" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="73" t="s">
-        <v>168</v>
+        <v>120</v>
       </c>
       <c r="B48" s="74">
-        <f>B46-0.4</f>
-        <v>0</v>
-      </c>
-      <c r="C48" s="74">
-        <v>0.3</v>
+        <f>B35</f>
+        <v>1</v>
+      </c>
+      <c r="C48" s="82" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="73" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="B49" s="74">
+        <f>B47-0.4</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="74">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="73" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" s="74">
         <v>20</v>
       </c>
-      <c r="C49" s="74">
+      <c r="C50" s="74">
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="37"/>
-      <c r="C50" s="8"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51" s="42"/>
-      <c r="C51" s="58"/>
+    <row r="51" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="37"/>
+      <c r="C51" s="8"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B52" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" s="24"/>
+      <c r="A52" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="42"/>
+      <c r="C52" s="58"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B53" s="43">
-        <v>2</v>
+        <v>35</v>
+      </c>
+      <c r="B53" s="43" t="s">
+        <v>4</v>
       </c>
       <c r="C53" s="24"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B54" s="43">
-        <f>B33</f>
-        <v>0.4</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>169</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C54" s="24"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="B55" s="43">
         <f>B34</f>
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="B56" s="43">
+        <f>B35</f>
         <v>1</v>
       </c>
-      <c r="C56" s="24">
-        <v>1</v>
+      <c r="C56" s="24" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="B57" s="43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C57" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>38</v>
+        <v>140</v>
       </c>
       <c r="B58" s="43">
-        <v>24</v>
-      </c>
-      <c r="C58" s="24"/>
+        <v>2</v>
+      </c>
+      <c r="C58" s="24">
+        <v>2</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B59" s="43">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C59" s="24"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>173</v>
+        <v>37</v>
       </c>
       <c r="B60" s="43">
-        <f>B30</f>
-        <v>30</v>
-      </c>
-      <c r="C60" s="24" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="37"/>
-      <c r="C61" s="8"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B62" s="44"/>
-      <c r="C62" s="59"/>
-    </row>
-    <row r="63" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B63" s="45">
-        <v>30</v>
-      </c>
-      <c r="C63" s="60"/>
+        <v>20</v>
+      </c>
+      <c r="C60" s="24"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B61" s="43">
+        <f>B31</f>
+        <v>0.5</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="37"/>
+      <c r="C62" s="8"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B63" s="44"/>
+      <c r="C63" s="59"/>
     </row>
     <row r="64" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B64" s="45" t="s">
-        <v>4</v>
+        <v>54</v>
+      </c>
+      <c r="B64" s="45">
+        <v>30</v>
       </c>
       <c r="C64" s="60"/>
     </row>
     <row r="65" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B65" s="45">
-        <v>3.05</v>
+        <v>55</v>
+      </c>
+      <c r="B65" s="45" t="s">
+        <v>4</v>
       </c>
       <c r="C65" s="60"/>
     </row>
     <row r="66" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="B66" s="45">
-        <v>20</v>
+        <v>3.05</v>
       </c>
       <c r="C66" s="60"/>
     </row>
     <row r="67" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B67" s="45">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C67" s="60"/>
     </row>
     <row r="68" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B68" s="45" t="s">
-        <v>4</v>
+        <v>57</v>
+      </c>
+      <c r="B68" s="45">
+        <v>31</v>
       </c>
       <c r="C68" s="60"/>
     </row>
     <row r="69" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B69" s="45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C69" s="60"/>
     </row>
     <row r="70" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B70" s="45">
-        <v>0.05</v>
+        <v>59</v>
+      </c>
+      <c r="B70" s="45" t="s">
+        <v>5</v>
       </c>
       <c r="C70" s="60"/>
     </row>
     <row r="71" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B71" s="45">
-        <v>3</v>
+        <v>0.05</v>
       </c>
       <c r="C71" s="60"/>
     </row>
     <row r="72" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B72" s="45" t="s">
-        <v>4</v>
+        <v>61</v>
+      </c>
+      <c r="B72" s="45">
+        <v>3</v>
       </c>
       <c r="C72" s="60"/>
     </row>
     <row r="73" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B73" s="45">
-        <v>1.4550000000000001</v>
+        <v>62</v>
+      </c>
+      <c r="B73" s="45" t="s">
+        <v>4</v>
       </c>
       <c r="C73" s="60"/>
     </row>
     <row r="74" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B74" s="45">
+        <v>1.4550000000000001</v>
+      </c>
+      <c r="C74" s="60"/>
+    </row>
+    <row r="75" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B75" s="45">
         <v>31</v>
-      </c>
-      <c r="C74" s="60"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B75" s="45" t="s">
-        <v>5</v>
       </c>
       <c r="C75" s="60"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B76" s="45">
-        <v>0.55500000000000005</v>
+        <v>65</v>
+      </c>
+      <c r="B76" s="45" t="s">
+        <v>5</v>
       </c>
       <c r="C76" s="60"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B77" s="45">
-        <v>0.5</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="C77" s="60"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B78" s="45">
-        <v>1.75</v>
+        <v>0.5</v>
       </c>
       <c r="C78" s="60"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B79" s="45" t="s">
-        <v>4</v>
+        <v>75</v>
+      </c>
+      <c r="B79" s="45">
+        <v>1.75</v>
       </c>
       <c r="C79" s="60"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="B80" s="45">
-        <v>4500</v>
+        <v>19</v>
+      </c>
+      <c r="B80" s="45" t="s">
+        <v>4</v>
       </c>
       <c r="C80" s="60"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="B81" s="45">
-        <v>50</v>
+        <v>4500</v>
       </c>
       <c r="C81" s="60"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="B82" s="45">
-        <v>100</v>
-      </c>
-      <c r="C82" s="60" t="s">
-        <v>203</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C82" s="60"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="20" t="s">
-        <v>223</v>
+        <v>181</v>
       </c>
       <c r="B83" s="45">
-        <v>0.9</v>
+        <v>100</v>
       </c>
       <c r="C83" s="60" t="s">
-        <v>224</v>
+        <v>182</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="20" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="B84" s="45">
-        <v>50</v>
+        <v>0.9</v>
       </c>
       <c r="C84" s="60" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="20" t="s">
-        <v>232</v>
+        <v>203</v>
       </c>
       <c r="B85" s="45">
+        <v>50</v>
+      </c>
+      <c r="C85" s="60" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="B86" s="45">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C85" s="60" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B87" s="47"/>
-      <c r="C87" s="26"/>
+      <c r="C86" s="60" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B88" s="48">
-        <v>0</v>
-      </c>
-      <c r="C88" s="28"/>
+      <c r="A88" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B88" s="47"/>
+      <c r="C88" s="26"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B89" s="48">
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="C89" s="28"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="27" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B90" s="48">
-        <v>-2</v>
+        <v>-12</v>
       </c>
       <c r="C90" s="28"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B91" s="48" t="s">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="B91" s="48">
+        <v>-2</v>
       </c>
       <c r="C91" s="28"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B92" s="48">
-        <v>-0.2</v>
+        <v>23</v>
+      </c>
+      <c r="B92" s="48" t="s">
+        <v>28</v>
       </c>
       <c r="C92" s="28"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="27" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B93" s="48">
-        <v>-1</v>
+        <v>-0.2</v>
       </c>
       <c r="C93" s="28"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="27" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B94" s="48">
         <v>-1</v>
@@ -4481,42 +4531,51 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B95" s="48">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C95" s="28"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="B96" s="48" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="B96" s="48">
+        <v>0</v>
       </c>
       <c r="C96" s="28"/>
     </row>
-    <row r="97" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97"/>
-      <c r="B97" s="46"/>
-      <c r="C97" s="5"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B98" s="49"/>
-      <c r="C98" s="29"/>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B97" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C97" s="28"/>
+    </row>
+    <row r="98" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98"/>
+      <c r="B98" s="46"/>
+      <c r="C98" s="5"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="11"/>
-      <c r="B99" s="50"/>
-      <c r="C99" s="32"/>
+      <c r="A99" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B99" s="49"/>
+      <c r="C99" s="29"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="11"/>
+      <c r="B100" s="50"/>
+      <c r="C100" s="32"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4529,8 +4588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4542,21 +4601,21 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="85" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="B2" s="69" t="s">
         <v>5</v>
@@ -4579,7 +4638,7 @@
     </row>
     <row r="3" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="85" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="B3" s="69" t="s">
         <v>4</v>
@@ -4602,7 +4661,7 @@
     </row>
     <row r="4" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="85" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="B4" s="69">
         <v>50</v>
@@ -4625,7 +4684,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="B5" s="69" t="s">
         <v>4</v>
@@ -4636,7 +4695,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B6" s="69" t="s">
         <v>4</v>
@@ -4645,12 +4704,12 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="B7" s="69" t="s">
         <v>4</v>
@@ -4661,7 +4720,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="B8" s="69" t="s">
         <v>4</v>
@@ -4672,7 +4731,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="B9" s="69" t="s">
         <v>4</v>
@@ -4683,7 +4742,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="B10" s="69" t="s">
         <v>4</v>
@@ -4694,7 +4753,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="B11" s="69" t="s">
         <v>4</v>
@@ -4705,7 +4764,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="B12" s="69" t="s">
         <v>4</v>
@@ -4714,12 +4773,12 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="B13" s="69" t="s">
         <v>4</v>
@@ -4730,7 +4789,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="B14" s="69" t="s">
         <v>4</v>
@@ -4741,7 +4800,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="B15" s="69" t="s">
         <v>4</v>
@@ -4752,7 +4811,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="B16" s="69" t="s">
         <v>4</v>
@@ -4763,7 +4822,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B17" s="69" t="s">
         <v>4</v>
@@ -4774,7 +4833,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="B18" s="69" t="s">
         <v>4</v>
@@ -4785,7 +4844,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="B19" s="69" t="s">
         <v>4</v>
@@ -4796,7 +4855,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="B20" s="69" t="s">
         <v>4</v>
@@ -4807,7 +4866,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="B21" s="69" t="s">
         <v>4</v>
@@ -4818,7 +4877,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="B22" s="69" t="s">
         <v>4</v>
@@ -4829,7 +4888,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="B23" s="69" t="s">
         <v>4</v>
@@ -4840,7 +4899,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="B24" s="69" t="s">
         <v>4</v>
@@ -4851,7 +4910,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="B25" s="69" t="s">
         <v>4</v>
@@ -4862,7 +4921,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="B26" s="69" t="s">
         <v>4</v>
@@ -4873,7 +4932,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="B27" s="69" t="s">
         <v>4</v>
@@ -4884,7 +4943,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
       <c r="B28" s="69" t="s">
         <v>4</v>
@@ -4895,7 +4954,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>229</v>
+        <v>207</v>
       </c>
       <c r="B29" s="69" t="s">
         <v>4</v>
@@ -4906,18 +4965,18 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="B30" s="69" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="69" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="B31" s="69" t="s">
         <v>4</v>
@@ -4928,7 +4987,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="B32" s="69" t="s">
         <v>4</v>
@@ -4939,7 +4998,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="B33" s="69" t="s">
         <v>4</v>
@@ -4950,60 +5009,746 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:C1">
-    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="19" priority="27" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C4">
-    <cfRule type="containsText" dxfId="15" priority="22" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C27">
-    <cfRule type="containsText" dxfId="14" priority="17" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28 C32:C33">
-    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="16" priority="10" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B31)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:C30">
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="C29">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B30">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="46" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="46" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="46" customWidth="1"/>
+    <col min="4" max="4" width="10" style="46" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="46" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="34">
+        <v>1</v>
+      </c>
+      <c r="B2" s="46">
+        <v>0.3</v>
+      </c>
+      <c r="C2" s="46">
+        <v>3</v>
+      </c>
+      <c r="D2" s="46">
+        <v>0.12</v>
+      </c>
+      <c r="E2" s="46">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F2" s="46">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="34">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="46">
+        <v>3</v>
+      </c>
+      <c r="D3" s="46">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="E3" s="46">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="F3" s="46">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="34">
+        <f t="shared" ref="A4:A67" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="46">
+        <v>12</v>
+      </c>
+      <c r="C4" s="46">
+        <v>12</v>
+      </c>
+      <c r="D4" s="46">
+        <v>7.8E-2</v>
+      </c>
+      <c r="E4" s="46">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="F4" s="46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="34">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="34">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="34">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="34">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="34">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="34">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="34">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="34">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="34">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="34">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="34">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="34">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="34">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="34">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="34">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="34">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="34">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="34">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="34">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="34">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="34">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="34">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="34">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="34">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="34">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="34">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="34">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="34">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="34">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="34">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="34">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="34">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="34">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="34">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="34">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="34">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="34">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="34">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="34">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="34">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="34">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="34">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="34">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="34">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="34">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="34">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="34">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="34">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="34">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="34">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="34">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="34">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="34">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="34">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="34">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="34">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="34">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="34">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="34">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="34">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="34">
+        <f t="shared" ref="A68:A100" si="1">A67+1</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="34">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="34">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="34">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="34">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="34">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="34">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="34">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="34">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="34">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="34">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="34">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="34">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="34">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="34">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="34">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="34">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="34">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="34">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="34">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="34">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="34">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="34">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="34">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="34">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="34">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="34">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="34">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="34">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="34">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="34">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="34">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="34">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>